<commit_message>
Waves didn't work; leaving this here so we have it before I get rid of them
</commit_message>
<xml_diff>
--- a/InstallationDemo/Assets/Manufacturing/assembly_manifest.xlsx
+++ b/InstallationDemo/Assets/Manufacturing/assembly_manifest.xlsx
@@ -1112,9 +1112,9 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="12.853482" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="13.567768" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="12.424911" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="12.835625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="13.335625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="11.210625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:3" s="1" customFormat="1">
@@ -1343,14 +1343,14 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="15.567768" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="6.567768" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="17.996339" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="27.853482" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="4.853482" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="4.996339" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="13.567768" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="12.424911" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="14.710625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="6.210625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="16.960625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="26.585625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="4.460625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="4.960625" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="13.335625" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="11.210625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:8" s="1" customFormat="1">
@@ -1798,14 +1798,14 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="15.567768" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="6.567768" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="17.996339" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="27.853482" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="4.853482" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="4.996339" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="13.567768" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="12.424911" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="14.710625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="6.210625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="16.960625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="26.585625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="4.460625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="4.960625" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="13.335625" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="11.210625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:8" s="1" customFormat="1">
@@ -2273,14 +2273,14 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="15.567768" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="6.567768" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="17.996339" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="27.853482" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="4.853482" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="4.996339" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="13.567768" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="12.424911" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="14.710625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="6.210625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="16.960625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="26.585625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="4.460625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="4.960625" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="13.335625" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="11.210625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:8" s="1" customFormat="1">
@@ -2748,14 +2748,14 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="15.567768" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="6.567768" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="17.996339" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="27.853482" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="4.282054" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="4.996339" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="13.567768" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="12.424911" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="14.710625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="6.210625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="16.960625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="26.585625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="4.335625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="4.960625" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="13.335625" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="11.210625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:8" s="1" customFormat="1">
@@ -3283,14 +3283,14 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="15.567768" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="6.567768" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="17.996339" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="27.853482" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="4.282054" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="4.996339" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="13.567768" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="12.424911" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="14.710625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="6.210625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="16.960625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="26.585625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="4.335625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="4.960625" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="13.335625" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="11.210625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:8" s="1" customFormat="1">
@@ -3778,14 +3778,14 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="15.567768" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="6.567768" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="17.996339" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="27.853482" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="4.853482" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="4.996339" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="13.567768" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="12.424911" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="14.710625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="6.210625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="16.960625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="26.585625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="4.460625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="4.960625" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="13.335625" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="11.210625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:8" s="1" customFormat="1">
@@ -4273,14 +4273,14 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="15.567768" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="6.567768" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="17.996339" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="27.853482" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="4.853482" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="4.996339" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="13.567768" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="12.424911" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="14.710625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="6.210625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="16.960625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="26.585625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="4.460625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="4.960625" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="13.335625" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="11.210625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:8" s="1" customFormat="1">
@@ -4768,14 +4768,14 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="15.567768" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="6.567768" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="17.996339" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="27.853482" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="4.853482" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="4.996339" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="13.567768" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="12.424911" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="14.710625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="6.210625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="16.960625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="26.585625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="4.460625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="4.960625" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="13.335625" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="11.210625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:8" s="1" customFormat="1">
@@ -5343,14 +5343,14 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="15.567768" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="6.567768" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="17.996339" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="27.853482" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="4.853482" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="4.996339" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="13.567768" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="12.424911" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="14.710625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="6.210625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="16.960625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="26.585625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="4.460625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="4.960625" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="13.335625" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="11.210625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:8" s="1" customFormat="1">
@@ -5898,14 +5898,14 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="15.567768" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="6.567768" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="17.996339" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="27.853482" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="4.282054" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="4.996339" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="13.567768" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="12.424911" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="14.710625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="6.210625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="16.960625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="26.585625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="4.335625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="4.960625" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="13.335625" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="11.210625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:8" s="1" customFormat="1">
@@ -6273,11 +6273,11 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="11.139196" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="4.996339" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="4.139196" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="10.424911" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="21.282054" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="10.710625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="4.835625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="3.960625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="10.210625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="20.710625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:5" s="1" customFormat="1">
@@ -6480,14 +6480,14 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="15.567768" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="6.567768" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="17.996339" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="27.853482" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="4.282054" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="4.996339" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="13.567768" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="12.424911" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="14.710625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="6.210625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="16.960625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="26.585625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="4.335625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="4.960625" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="13.335625" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="11.210625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:8" s="1" customFormat="1">
@@ -6995,14 +6995,14 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="15.567768" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="6.567768" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="17.996339" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="27.853482" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="4.853482" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="4.996339" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="13.567768" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="12.424911" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="14.710625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="6.210625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="16.960625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="26.585625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="4.460625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="4.960625" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="13.335625" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="11.210625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:8" s="1" customFormat="1">
@@ -7550,14 +7550,14 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="15.567768" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="6.567768" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="17.996339" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="27.853482" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="4.853482" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="4.996339" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="13.567768" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="12.424911" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="14.710625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="6.210625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="16.960625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="26.585625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="4.460625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="4.960625" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="13.335625" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="11.210625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:8" s="1" customFormat="1">
@@ -7985,14 +7985,14 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="15.567768" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="6.567768" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="17.996339" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="27.853482" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="4.853482" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="4.996339" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="13.567768" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="12.424911" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="14.710625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="6.210625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="16.960625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="26.585625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="4.460625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="4.960625" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="13.335625" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="11.210625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:8" s="1" customFormat="1">
@@ -8460,14 +8460,14 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="15.567768" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="6.567768" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="17.996339" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="27.853482" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="4.853482" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="4.996339" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="13.567768" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="12.424911" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="14.710625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="6.210625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="16.960625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="26.585625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="4.460625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="4.960625" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="13.335625" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="11.210625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:8" s="1" customFormat="1">
@@ -8875,14 +8875,14 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="15.567768" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="6.567768" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="17.996339" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="27.853482" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="4.853482" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="4.996339" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="13.567768" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="12.424911" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="14.710625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="6.210625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="16.960625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="26.585625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="4.460625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="4.960625" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="13.335625" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="11.210625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:8" s="1" customFormat="1">
@@ -9330,14 +9330,14 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="15.567768" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="6.567768" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="17.996339" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="27.853482" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="4.853482" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="4.996339" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="13.567768" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="12.424911" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="14.710625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="6.210625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="16.960625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="26.585625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="4.460625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="4.960625" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="13.335625" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="11.210625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:8" s="1" customFormat="1">

</xml_diff>